<commit_message>
build out weighting code to point where demo weights can be applied to sum scores
</commit_message>
<xml_diff>
--- a/INPUT-FILES/NORMS/TOD-E demographic variable labels.xlsx
+++ b/INPUT-FILES/NORMS/TOD-E demographic variable labels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklein\Desktop\TOD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/TOD-R/INPUT-FILES/NORMS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCCECBF-0741-4742-914B-DAC3F8FC1BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179A4929-1ACA-F744-AB4C-E74F53AECBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C924A35-86B4-4486-8783-609F2044D53F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4C924A35-86B4-4486-8783-609F2044D53F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,19 +541,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92527B5A-57BB-4605-BF8E-2CC2875775F6}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -561,12 +564,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -574,7 +577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -582,12 +585,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -595,7 +598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -603,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -611,7 +614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -619,12 +622,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -632,7 +635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -640,7 +643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -648,7 +651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -659,7 +662,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
@@ -667,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -675,7 +678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -683,12 +686,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -696,7 +699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -704,7 +707,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -712,7 +715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -720,12 +723,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -733,7 +736,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -741,7 +744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3</v>
       </c>
@@ -749,7 +752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -757,7 +760,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>5</v>
       </c>
@@ -765,7 +768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>6</v>
       </c>
@@ -773,7 +776,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>7</v>
       </c>
@@ -781,7 +784,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>8</v>
       </c>
@@ -789,12 +792,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -802,7 +805,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
@@ -810,7 +813,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -818,7 +821,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4</v>
       </c>
@@ -826,7 +829,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -834,7 +837,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>6</v>
       </c>
@@ -844,7 +847,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>